<commit_message>
fixed bugs, improved stability
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -399,12 +399,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Email</v>
+        <v>Test</v>
       </c>
       <c r="B1" t="str">
         <v>Name</v>

</xml_diff>